<commit_message>
sredjen logout, redirekcija, preuzimanje izvestaja
</commit_message>
<xml_diff>
--- a/simulacije-Backend/templates/template1.xlsx
+++ b/simulacije-Backend/templates/template1.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Name</t>
   </si>
@@ -22,22 +22,34 @@
     <t>E-mail</t>
   </si>
   <si>
+    <t>Score</t>
+  </si>
+  <si>
+    <t>${table:user.name}</t>
+  </si>
+  <si>
+    <t>${table:user.email}</t>
+  </si>
+  <si>
+    <t>${table:user.score}</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>${table:user.age}</t>
+  </si>
+  <si>
     <t>Registration date</t>
   </si>
   <si>
-    <t>Score</t>
-  </si>
-  <si>
-    <t>${table:users.name}</t>
-  </si>
-  <si>
-    <t>${table:users.email}</t>
-  </si>
-  <si>
-    <t>${table:users.score}</t>
-  </si>
-  <si>
-    <t>${table:users.registrationDate}</t>
+    <t>${table:user.registrationDate}</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>${table:user.role}</t>
   </si>
 </sst>
 </file>
@@ -135,7 +147,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -170,7 +182,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -379,21 +391,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.140625" customWidth="1"/>
-    <col min="2" max="2" width="32.85546875" customWidth="1"/>
-    <col min="3" max="3" width="36.5703125" customWidth="1"/>
-    <col min="4" max="4" width="9" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" customWidth="1"/>
+    <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -404,21 +416,33 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
-        <v>6</v>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>